<commit_message>
Finalizando Desenvolvimento do Banco de Dados
</commit_message>
<xml_diff>
--- a/Escopo/Modelos/Especialidades.xlsx
+++ b/Escopo/Modelos/Especialidades.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D086AD-3A39-483E-9ADF-AB4C011ABA0C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -81,17 +82,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -125,11 +118,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,165 +401,162 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>